<commit_message>
added cmd shell executability added removeResultsAndDiags before invocation improved error handling
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470"/>
+    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,13 @@
   <definedNames>
     <definedName name="R_Addin" localSheetId="1">Input_Toy!$J$1:$L$5</definedName>
     <definedName name="R_Addin">Input!$J$11:$L$15</definedName>
-    <definedName name="R_AddinAnotherDef" localSheetId="1">Input_Toy!$J$7:$L$11</definedName>
+    <definedName name="R_AddinAnotherDef" localSheetId="1">Input_Toy!$J$7:$L$12</definedName>
     <definedName name="R_AddinAnotherDef">Input!$M$11:$O$15</definedName>
     <definedName name="test_in" localSheetId="1">Input_Toy!$B$1:$H$3</definedName>
     <definedName name="test_in">Input!$B$1:$H$306</definedName>
     <definedName name="test_out" localSheetId="1">Input_Toy!$A$1:$A$3</definedName>
     <definedName name="test_out">Input!$A$2:$A$49</definedName>
-    <definedName name="testdiagram" localSheetId="1">Input_Toy!$J$16</definedName>
+    <definedName name="testdiagram" localSheetId="1">Input_Toy!$J$17</definedName>
     <definedName name="testdiagram">Input!$J$19</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="34">
   <si>
     <t/>
   </si>
@@ -121,6 +121,15 @@
   <si>
     <t>testRDir</t>
   </si>
+  <si>
+    <t>rexec</t>
+  </si>
+  <si>
+    <t>cmd</t>
+  </si>
+  <si>
+    <t>testStartRscript.cmd</t>
+  </si>
 </sst>
 </file>
 
@@ -155,18 +164,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -186,7 +189,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -194,7 +197,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
@@ -268,7 +270,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Grafik 5"/>
+        <xdr:cNvPr id="3" name="Grafik 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -288,55 +290,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3295650" y="2914650"/>
-          <a:ext cx="4572000" cy="4572000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Grafik 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2943225" y="2390775"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -639,8 +592,8 @@
   <sheetPr codeName="eingabe"/>
   <dimension ref="A1:O306"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -702,8 +655,8 @@
       <c r="H2" s="1">
         <v>0.40250000000000002</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="7"/>
+      <c r="J2" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -732,8 +685,8 @@
       <c r="H3" s="1">
         <v>0.50719999999999998</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="7"/>
+      <c r="J3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -762,8 +715,8 @@
       <c r="H4" s="1">
         <v>1.7100000000000001E-2</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8" t="s">
+      <c r="I4" s="7"/>
+      <c r="J4" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -792,8 +745,8 @@
       <c r="H5" s="1">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8" t="s">
+      <c r="I5" s="7"/>
+      <c r="J5" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -822,8 +775,8 @@
       <c r="H6" s="1">
         <v>0.28749999999999998</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8" t="s">
+      <c r="I6" s="7"/>
+      <c r="J6" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -852,12 +805,12 @@
       <c r="H7" s="1">
         <v>8.8999999999999999E-3</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8" t="s">
+      <c r="I7" s="7"/>
+      <c r="J7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -884,12 +837,12 @@
       <c r="H8" s="1">
         <v>1.15E-2</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8" t="s">
+      <c r="I8" s="7"/>
+      <c r="J8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -916,7 +869,7 @@
       <c r="H9" s="1">
         <v>1.61E-2</v>
       </c>
-      <c r="I9" s="8"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -943,7 +896,7 @@
       <c r="H10" s="1">
         <v>3.1099999999999999E-2</v>
       </c>
-      <c r="I10" s="8"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -970,7 +923,7 @@
       <c r="H11" s="1">
         <v>0.63400000000000001</v>
       </c>
-      <c r="I11" s="8"/>
+      <c r="I11" s="7"/>
       <c r="J11" s="4" t="s">
         <v>2</v>
       </c>
@@ -1009,7 +962,7 @@
       <c r="H12" s="1">
         <v>0.5706</v>
       </c>
-      <c r="I12" s="8"/>
+      <c r="I12" s="7"/>
       <c r="J12" s="3" t="s">
         <v>1</v>
       </c>
@@ -1051,7 +1004,7 @@
       <c r="H13" s="1">
         <v>2.4E-2</v>
       </c>
-      <c r="I13" s="8"/>
+      <c r="I13" s="7"/>
       <c r="J13" s="3" t="s">
         <v>6</v>
       </c>
@@ -1093,7 +1046,7 @@
       <c r="H14" s="1">
         <v>2.4E-2</v>
       </c>
-      <c r="I14" s="8"/>
+      <c r="I14" s="7"/>
       <c r="J14" s="3" t="s">
         <v>5</v>
       </c>
@@ -1135,7 +1088,7 @@
       <c r="H15" s="1">
         <v>1.38E-2</v>
       </c>
-      <c r="I15" s="8"/>
+      <c r="I15" s="7"/>
       <c r="J15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1177,10 +1130,10 @@
       <c r="H16" s="1">
         <v>0.40250000000000002</v>
       </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -1207,10 +1160,10 @@
       <c r="H17" s="1">
         <v>0.40250000000000002</v>
       </c>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -1237,10 +1190,10 @@
       <c r="H18" s="1">
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -1267,10 +1220,10 @@
       <c r="H19" s="1">
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -1297,10 +1250,10 @@
       <c r="H20" s="1">
         <v>1.61E-2</v>
       </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -1327,10 +1280,10 @@
       <c r="H21" s="1">
         <v>2.3E-2</v>
       </c>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -1357,10 +1310,10 @@
       <c r="H22" s="1">
         <v>2.5899999999999999E-2</v>
       </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -1387,10 +1340,10 @@
       <c r="H23" s="1">
         <v>5.7500000000000002E-2</v>
       </c>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -1417,10 +1370,10 @@
       <c r="H24" s="1">
         <v>5.1799999999999999E-2</v>
       </c>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -1447,10 +1400,10 @@
       <c r="H25" s="1">
         <v>0.73540000000000005</v>
       </c>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -1477,10 +1430,10 @@
       <c r="H26" s="1">
         <v>0.54520000000000002</v>
       </c>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -1507,10 +1460,10 @@
       <c r="H27" s="1">
         <v>0.59589999999999999</v>
       </c>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -1537,10 +1490,10 @@
       <c r="H28" s="1">
         <v>0.317</v>
       </c>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -1567,10 +1520,10 @@
       <c r="H29" s="1">
         <v>3.0499999999999999E-2</v>
       </c>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -1597,10 +1550,10 @@
       <c r="H30" s="1">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -1627,10 +1580,10 @@
       <c r="H31" s="1">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -1657,10 +1610,10 @@
       <c r="H32" s="1">
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -1687,10 +1640,10 @@
       <c r="H33" s="1">
         <v>0.46</v>
       </c>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
@@ -1717,10 +1670,10 @@
       <c r="H34" s="1">
         <v>0.34499999999999997</v>
       </c>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
@@ -1747,10 +1700,10 @@
       <c r="H35" s="1">
         <v>0.34499999999999997</v>
       </c>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
@@ -1777,10 +1730,10 @@
       <c r="H36" s="1">
         <v>0.115</v>
       </c>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
@@ -1807,10 +1760,10 @@
       <c r="H37" s="1">
         <v>1.9E-2</v>
       </c>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
@@ -1837,10 +1790,10 @@
       <c r="H38" s="1">
         <v>1.0800000000000001E-2</v>
       </c>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
@@ -1867,10 +1820,10 @@
       <c r="H39" s="1">
         <v>1.0800000000000001E-2</v>
       </c>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
@@ -1897,10 +1850,10 @@
       <c r="H40" s="1">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
@@ -1927,10 +1880,10 @@
       <c r="H41" s="1">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
@@ -1957,10 +1910,10 @@
       <c r="H42" s="1">
         <v>2.3E-2</v>
       </c>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
@@ -1987,10 +1940,10 @@
       <c r="H43" s="1">
         <v>2.01E-2</v>
       </c>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
@@ -2017,10 +1970,10 @@
       <c r="H44" s="1">
         <v>1.15E-2</v>
       </c>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
@@ -2047,10 +2000,10 @@
       <c r="H45" s="1">
         <v>8.0500000000000002E-2</v>
       </c>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
@@ -2077,10 +2030,10 @@
       <c r="H46" s="1">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
@@ -2107,10 +2060,10 @@
       <c r="H47" s="1">
         <v>4.8899999999999999E-2</v>
       </c>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
@@ -2137,10 +2090,10 @@
       <c r="H48" s="1">
         <v>2.3E-2</v>
       </c>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49"/>
@@ -2165,8 +2118,8 @@
       <c r="H49" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
@@ -2190,7 +2143,7 @@
       <c r="H50" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I50" s="8"/>
+      <c r="I50" s="7"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
@@ -8093,10 +8046,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="eingabeToy"/>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8110,9 +8063,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>3</v>
-      </c>
+      <c r="A1"/>
       <c r="B1">
         <v>23</v>
       </c>
@@ -8143,9 +8094,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>3</v>
-      </c>
+      <c r="A2"/>
       <c r="B2">
         <v>3</v>
       </c>
@@ -8211,7 +8160,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
+      <c r="A4"/>
       <c r="J4" s="3" t="s">
         <v>5</v>
       </c>
@@ -8220,7 +8169,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5"/>
       <c r="J5" s="3" t="s">
         <v>7</v>
       </c>
@@ -8229,75 +8178,168 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="A6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7"/>
       <c r="C7" s="6"/>
       <c r="J7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8"/>
+      <c r="J8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="J8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+      <c r="A9"/>
       <c r="J9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10"/>
+      <c r="J10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="J10" s="3" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11"/>
+      <c r="J11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="J11" s="3" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12"/>
+      <c r="J12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-    </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
+      <c r="A13"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
+      <c r="A14"/>
       <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
+      <c r="A15"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
+      <c r="A16"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
+      <c r="A17"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
+      <c r="A18"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47"/>
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -8305,6 +8347,5 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;Z&amp;F&amp;A</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>